<commit_message>
fix: update pv-reception to list all target depots
</commit_message>
<xml_diff>
--- a/client/src/assets/pv-reception.xlsx
+++ b/client/src/assets/pv-reception.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jniles\Desktop\odk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB207EA-1EDC-44AB-8FDB-D79BA8166609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7725ED-D413-4B36-80C2-5AA90E3C1EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{ACEB9501-F7B9-4F65-B30E-DBD646EB7FDB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{ACEB9501-F7B9-4F65-B30E-DBD646EB7FDB}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="108">
   <si>
     <t>type</t>
   </si>
@@ -197,9 +197,6 @@
     <t>flux_id</t>
   </si>
   <si>
-    <t>search('lots')</t>
-  </si>
-  <si>
     <t>Nombre des articles</t>
   </si>
   <si>
@@ -344,7 +341,25 @@
     <t>Entity Uuid</t>
   </si>
   <si>
-    <t>pulldata('transfers','target_depot_uuid','document_uuid',${document_uuid})</t>
+    <t>pulldata('transfers','origin_depot_uuid','document_uuid',${document_uuid})</t>
+  </si>
+  <si>
+    <t>unit_cost</t>
+  </si>
+  <si>
+    <t>Unit Cost</t>
+  </si>
+  <si>
+    <t>pulldata(‘lots','unit_cost','barcode',${barcode})</t>
+  </si>
+  <si>
+    <t>search('transfers')</t>
+  </si>
+  <si>
+    <t>target_depot_uuid</t>
+  </si>
+  <si>
+    <t>target_depot_text</t>
   </si>
 </sst>
 </file>
@@ -623,7 +638,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{E6B416BE-EC4C-4554-927F-A7B686A8EC19}"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1034,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F07FD78-1BE8-4A7B-8986-3A458432F6AF}">
-  <dimension ref="A1:O47"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,7 +1212,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="30"/>
@@ -1188,7 +1223,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -1219,7 +1254,7 @@
         <v>52</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="30"/>
@@ -1255,16 +1290,16 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>49</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>21</v>
@@ -1277,23 +1312,23 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="E10" s="32" t="s">
         <v>21</v>
@@ -1306,7 +1341,7 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
@@ -1316,10 +1351,10 @@
         <v>24</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>100</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>101</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="36"/>
@@ -1329,7 +1364,7 @@
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
@@ -1352,7 +1387,7 @@
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
@@ -1370,7 +1405,7 @@
         <v>27</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E13" s="34" t="s">
         <v>21</v>
@@ -1391,13 +1426,13 @@
         <v>28</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E14" s="34" t="s">
         <v>21</v>
@@ -1422,10 +1457,10 @@
         <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="31"/>
@@ -1434,7 +1469,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -1450,10 +1485,10 @@
         <v>32</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>21</v>
@@ -1485,7 +1520,7 @@
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
@@ -1500,7 +1535,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="37" t="s">
@@ -1510,7 +1545,7 @@
         <v>35</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
@@ -1526,10 +1561,10 @@
         <v>24</v>
       </c>
       <c r="B19" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>88</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>89</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="36"/>
@@ -1541,7 +1576,7 @@
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
@@ -1556,7 +1591,7 @@
         <v>23</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="36"/>
@@ -1568,7 +1603,7 @@
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
@@ -1583,7 +1618,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="36"/>
@@ -1595,7 +1630,7 @@
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
@@ -1607,10 +1642,10 @@
         <v>24</v>
       </c>
       <c r="B22" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>91</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>92</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="36"/>
@@ -1622,7 +1657,7 @@
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
@@ -1634,10 +1669,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>69</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="36"/>
@@ -1649,119 +1684,129 @@
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
     </row>
-    <row r="24" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+    </row>
+    <row r="25" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="38"/>
-      <c r="E24" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="B25" s="38"/>
+      <c r="C25" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="38"/>
+      <c r="E25" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="12"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="B27" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="12"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B28" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="13"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="1"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="13"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
@@ -1829,6 +1874,7 @@
       <c r="L32" s="14"/>
       <c r="M32" s="14"/>
       <c r="N32" s="14"/>
+      <c r="O32" s="1"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
@@ -2070,16 +2116,40 @@
       <c r="M47" s="14"/>
       <c r="N47" s="14"/>
     </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E8 E10 E23:E25 E12:E20">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+  <conditionalFormatting sqref="E2:E8 E10 E23 E12:E20 E25:E26">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"no"</formula>
     </cfRule>
@@ -2087,7 +2157,7 @@
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
+  <conditionalFormatting sqref="E22">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"no"</formula>
     </cfRule>
@@ -2095,7 +2165,7 @@
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
+  <conditionalFormatting sqref="E11">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"no"</formula>
     </cfRule>
@@ -2103,7 +2173,7 @@
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
+  <conditionalFormatting sqref="E24">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"no"</formula>
     </cfRule>
@@ -2119,8 +2189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABCE083-D538-4915-90FA-0F031077E4CF}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2173,18 +2243,18 @@
         <v>51</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>49</v>
+        <v>106</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="23" t="s">
         <v>2</v>
@@ -2234,16 +2304,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>55</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>56</v>
       </c>
       <c r="C2" s="26">
         <v>1</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix typos and allow auto-send for odk
</commit_message>
<xml_diff>
--- a/client/src/assets/pv-reception.xlsx
+++ b/client/src/assets/pv-reception.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jniles\Desktop\odk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRUCE XPS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7725ED-D413-4B36-80C2-5AA90E3C1EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCF3385-67B0-49A0-BB2E-C4360D2D4560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{ACEB9501-F7B9-4F65-B30E-DBD646EB7FDB}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="14136" xr2:uid="{ACEB9501-F7B9-4F65-B30E-DBD646EB7FDB}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -269,21 +269,12 @@
     <t>Flux</t>
   </si>
   <si>
-    <t>Veuillez selectionner le FOSA pour l'entre de stock</t>
-  </si>
-  <si>
     <t>select_one transfers</t>
   </si>
   <si>
-    <t>Veuillez selectionner le numero du bon d'expedition</t>
-  </si>
-  <si>
     <t>Le bon d'expedition est sur le format SM.XX.YYY</t>
   </si>
   <si>
-    <t>La reception de produit devrait se faire sur place a la formation sanitaire.</t>
-  </si>
-  <si>
     <t>transfers</t>
   </si>
   <si>
@@ -317,9 +308,6 @@
     <t>pulldata(‘lots','group_name','barcode',${barcode})</t>
   </si>
   <si>
-    <t>Vous avez preciser ${label} de l'article ${text} (${inventory_group}).</t>
-  </si>
-  <si>
     <t>search('transfers',  'matches','target_depot_uuid', ${depot_uuid})</t>
   </si>
   <si>
@@ -360,6 +348,18 @@
   </si>
   <si>
     <t>target_depot_text</t>
+  </si>
+  <si>
+    <t>Vous avez precisé ${label} de l'article ${text} (${inventory_group}).</t>
+  </si>
+  <si>
+    <t>La réception de produit devrait se faire sur place à la formation sanitaire.</t>
+  </si>
+  <si>
+    <t>Veuillez sélectionner la FOSA pour l'entrée de stock</t>
+  </si>
+  <si>
+    <t>Veuillez sélectionner le numéro du bon d'expédition</t>
   </si>
 </sst>
 </file>
@@ -773,7 +773,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1071,30 +1071,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F07FD78-1BE8-4A7B-8986-3A458432F6AF}">
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.41796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.15625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.26171875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.26171875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.83984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -1162,7 +1162,7 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1183,7 +1183,7 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -1204,7 +1204,7 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -1223,13 +1223,13 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="25"/>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
@@ -1246,7 +1246,7 @@
       <c r="N6" s="25"/>
       <c r="O6" s="25"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="25" t="s">
         <v>22</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="25"/>
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
@@ -1288,7 +1288,7 @@
       <c r="N8" s="25"/>
       <c r="O8" s="25"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6" t="s">
         <v>65</v>
       </c>
@@ -1296,10 +1296,10 @@
         <v>49</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>21</v>
@@ -1312,23 +1312,23 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>64</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E10" s="32" t="s">
         <v>21</v>
@@ -1341,20 +1341,20 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="36"/>
@@ -1364,14 +1364,14 @@
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="7" t="s">
         <v>22</v>
       </c>
@@ -1387,14 +1387,14 @@
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8" t="s">
         <v>25</v>
       </c>
@@ -1421,7 +1421,7 @@
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="8" t="s">
         <v>28</v>
       </c>
@@ -1452,7 +1452,7 @@
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="5" t="s">
         <v>31</v>
       </c>
@@ -1477,7 +1477,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="9" t="s">
         <v>32</v>
       </c>
@@ -1504,7 +1504,7 @@
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="10" t="s">
         <v>24</v>
       </c>
@@ -1520,14 +1520,14 @@
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="11" t="s">
         <v>19</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>35</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
@@ -1556,15 +1556,15 @@
       <c r="N18" s="11"/>
       <c r="O18" s="11"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="36"/>
@@ -1576,14 +1576,14 @@
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="10" t="s">
         <v>24</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>23</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="36"/>
@@ -1603,14 +1603,14 @@
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="10" t="s">
         <v>24</v>
       </c>
@@ -1637,15 +1637,15 @@
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="36"/>
@@ -1657,14 +1657,14 @@
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="10" t="s">
         <v>24</v>
       </c>
@@ -1691,15 +1691,15 @@
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="36"/>
@@ -1711,24 +1711,24 @@
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
     </row>
-    <row r="25" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="38" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="38"/>
       <c r="C25" s="38" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="D25" s="38"/>
       <c r="E25" s="39" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F25" s="38"/>
       <c r="G25" s="38"/>
@@ -1741,7 +1741,7 @@
       <c r="N25" s="38"/>
       <c r="O25" s="38"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="5" t="s">
         <v>37</v>
       </c>
@@ -1760,7 +1760,7 @@
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="8" t="s">
         <v>24</v>
       </c>
@@ -1783,7 +1783,7 @@
       <c r="N27" s="8"/>
       <c r="O27" s="12"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
@@ -1795,7 +1795,7 @@
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -1808,7 +1808,7 @@
       <c r="N28" s="4"/>
       <c r="O28" s="13"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -1825,7 +1825,7 @@
       <c r="N29" s="14"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="14"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -1842,7 +1842,7 @@
       <c r="N30" s="14"/>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="14"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
@@ -1859,7 +1859,7 @@
       <c r="N31" s="14"/>
       <c r="O31" s="1"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -1876,7 +1876,7 @@
       <c r="N32" s="14"/>
       <c r="O32" s="1"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -1892,7 +1892,7 @@
       <c r="M33" s="14"/>
       <c r="N33" s="14"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="14"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -1908,7 +1908,7 @@
       <c r="M34" s="14"/>
       <c r="N34" s="14"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -1924,7 +1924,7 @@
       <c r="M35" s="14"/>
       <c r="N35" s="14"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -1940,7 +1940,7 @@
       <c r="M36" s="14"/>
       <c r="N36" s="14"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -1956,7 +1956,7 @@
       <c r="M37" s="14"/>
       <c r="N37" s="14"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="14"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -1972,7 +1972,7 @@
       <c r="M38" s="14"/>
       <c r="N38" s="14"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -1988,7 +1988,7 @@
       <c r="M39" s="14"/>
       <c r="N39" s="14"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="14"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -2004,7 +2004,7 @@
       <c r="M40" s="14"/>
       <c r="N40" s="14"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="14"/>
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
@@ -2020,7 +2020,7 @@
       <c r="M41" s="14"/>
       <c r="N41" s="14"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="14"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -2036,7 +2036,7 @@
       <c r="M42" s="14"/>
       <c r="N42" s="14"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="14"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -2052,7 +2052,7 @@
       <c r="M43" s="14"/>
       <c r="N43" s="14"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="14"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -2068,7 +2068,7 @@
       <c r="M44" s="14"/>
       <c r="N44" s="14"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -2084,7 +2084,7 @@
       <c r="M45" s="14"/>
       <c r="N45" s="14"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="14"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -2100,7 +2100,7 @@
       <c r="M46" s="14"/>
       <c r="N46" s="14"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="14"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
@@ -2116,7 +2116,7 @@
       <c r="M47" s="14"/>
       <c r="N47" s="14"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="14"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
@@ -2189,18 +2189,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABCE083-D538-4915-90FA-0F031077E4CF}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="15" t="s">
         <v>39</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="26" t="s">
         <v>40</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26" t="s">
         <v>40</v>
       </c>
@@ -2233,25 +2233,25 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="20"/>
       <c r="B4" s="21"/>
       <c r="C4" s="22"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="18" t="s">
         <v>51</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>64</v>
@@ -2260,7 +2260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="24"/>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
@@ -2279,16 +2279,16 @@
       <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.15625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A1" s="27" t="s">
         <v>45</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="26" t="s">
         <v>54</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2546,18 +2546,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2580,6 +2580,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0824729E-DE7E-4F3F-9D34-71271A92735C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{284D7670-C02C-411E-B168-4D15B1D029F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2594,12 +2602,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0824729E-DE7E-4F3F-9D34-71271A92735C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>